<commit_message>
tidied Flask and Django demos
</commit_message>
<xml_diff>
--- a/src/16 Scientific Libraries/06 Spreadsheets/data/calendar.xlsx
+++ b/src/16 Scientific Libraries/06 Spreadsheets/data/calendar.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
     <col width="4" customWidth="1" min="2" max="2"/>
     <col width="4" customWidth="1" min="3" max="3"/>
     <col width="4" customWidth="1" min="4" max="4"/>
@@ -435,47 +434,47 @@
     <col width="4" customWidth="1" min="6" max="6"/>
     <col width="4" customWidth="1" min="7" max="7"/>
     <col width="4" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="12" customWidth="1" min="14" max="14"/>
-    <col width="12" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="12" customWidth="1" min="18" max="18"/>
-    <col width="12" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="12" customWidth="1" min="21" max="21"/>
-    <col width="12" customWidth="1" min="22" max="22"/>
-    <col width="12" customWidth="1" min="23" max="23"/>
-    <col width="12" customWidth="1" min="24" max="24"/>
-    <col width="12" customWidth="1" min="25" max="25"/>
-    <col width="12" customWidth="1" min="26" max="26"/>
-    <col width="12" customWidth="1" min="27" max="27"/>
-    <col width="12" customWidth="1" min="28" max="28"/>
-    <col width="12" customWidth="1" min="29" max="29"/>
-    <col width="12" customWidth="1" min="30" max="30"/>
-    <col width="12" customWidth="1" min="31" max="31"/>
-    <col width="12" customWidth="1" min="32" max="32"/>
-    <col width="12" customWidth="1" min="33" max="33"/>
-    <col width="12" customWidth="1" min="34" max="34"/>
-    <col width="12" customWidth="1" min="35" max="35"/>
-    <col width="12" customWidth="1" min="36" max="36"/>
-    <col width="12" customWidth="1" min="37" max="37"/>
-    <col width="12" customWidth="1" min="38" max="38"/>
-    <col width="12" customWidth="1" min="39" max="39"/>
-    <col width="12" customWidth="1" min="40" max="40"/>
-    <col width="12" customWidth="1" min="41" max="41"/>
-    <col width="12" customWidth="1" min="42" max="42"/>
-    <col width="12" customWidth="1" min="43" max="43"/>
-    <col width="12" customWidth="1" min="44" max="44"/>
-    <col width="12" customWidth="1" min="45" max="45"/>
-    <col width="12" customWidth="1" min="46" max="46"/>
-    <col width="12" customWidth="1" min="47" max="47"/>
-    <col width="12" customWidth="1" min="48" max="48"/>
-    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="24" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="10" max="10"/>
+    <col width="24" customWidth="1" min="11" max="11"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
+    <col width="24" customWidth="1" min="13" max="13"/>
+    <col width="24" customWidth="1" min="14" max="14"/>
+    <col width="24" customWidth="1" min="15" max="15"/>
+    <col width="24" customWidth="1" min="16" max="16"/>
+    <col width="24" customWidth="1" min="17" max="17"/>
+    <col width="24" customWidth="1" min="18" max="18"/>
+    <col width="24" customWidth="1" min="19" max="19"/>
+    <col width="24" customWidth="1" min="20" max="20"/>
+    <col width="24" customWidth="1" min="21" max="21"/>
+    <col width="24" customWidth="1" min="22" max="22"/>
+    <col width="24" customWidth="1" min="23" max="23"/>
+    <col width="24" customWidth="1" min="24" max="24"/>
+    <col width="24" customWidth="1" min="25" max="25"/>
+    <col width="24" customWidth="1" min="26" max="26"/>
+    <col width="24" customWidth="1" min="27" max="27"/>
+    <col width="24" customWidth="1" min="28" max="28"/>
+    <col width="24" customWidth="1" min="29" max="29"/>
+    <col width="24" customWidth="1" min="30" max="30"/>
+    <col width="24" customWidth="1" min="31" max="31"/>
+    <col width="24" customWidth="1" min="32" max="32"/>
+    <col width="24" customWidth="1" min="33" max="33"/>
+    <col width="24" customWidth="1" min="34" max="34"/>
+    <col width="24" customWidth="1" min="35" max="35"/>
+    <col width="24" customWidth="1" min="36" max="36"/>
+    <col width="24" customWidth="1" min="37" max="37"/>
+    <col width="24" customWidth="1" min="38" max="38"/>
+    <col width="24" customWidth="1" min="39" max="39"/>
+    <col width="24" customWidth="1" min="40" max="40"/>
+    <col width="24" customWidth="1" min="41" max="41"/>
+    <col width="24" customWidth="1" min="42" max="42"/>
+    <col width="24" customWidth="1" min="43" max="43"/>
+    <col width="24" customWidth="1" min="44" max="44"/>
+    <col width="24" customWidth="1" min="45" max="45"/>
+    <col width="24" customWidth="1" min="46" max="46"/>
+    <col width="24" customWidth="1" min="47" max="47"/>
+    <col width="24" customWidth="1" min="48" max="48"/>
+    <col width="24" customWidth="1" min="49" max="49"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">

</xml_diff>